<commit_message>
For different width of magnets
Will try to vary the ratio of magnets
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A10:A10"/>
+  <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,9 +421,69 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>22.11762717781596</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>33.9660272262802</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>43.60027209447989</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>50.54485097393651</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>55.34780330285171</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>57.55476682982366</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>58.50349776193204</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>58.35476861619483</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>57.42914312388932</v>
+      </c>
+    </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>45.94893874692611</v>
+        <v>56.06356341679849</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>54.30225190802328</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>52.48656516387938</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>50.45953388201623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
try to find the best steel width and magnet width
put the functions out of the loops. change some variable names. 大但设想，小心求证。
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -1,34 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\226\pyfemm---magnetic-couplings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF546414-56B7-4AB7-B43E-F48602662B0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <name val="Calibri"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -47,80 +58,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,85 +360,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A1:A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n">
-        <v>22.11762717781596</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>33.9660272262802</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>43.60027209447989</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>50.54485097393651</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>55.34780330285171</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>57.55476682982366</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>58.50349776193204</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>58.35476861619483</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>57.42914312388932</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>56.06356341679849</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>54.30225190802328</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>52.48656516387938</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>50.45953388201623</v>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>20.509667548414669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>32.996854167476243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>43.386692889998827</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>51.031519556059713</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>55.990247618994637</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>58.754609883378777</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>59.723328156581744</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>59.585625839143709</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>58.617002916750529</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>57.264071658810472</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>55.676311540653167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>53.896639957984988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>51.990082851649042</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
The maximum torque has been found
The maximum torque is at (4,3600).
Maybe repeat the steps to get more accurate value.
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -1,45 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\226\pyfemm---magnetic-couplings\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF546414-56B7-4AB7-B43E-F48602662B0B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5508" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -58,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -360,82 +408,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:A14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A70:A94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A1:A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>20.509667548414669</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>32.996854167476243</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>43.386692889998827</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>51.031519556059713</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>55.990247618994637</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>58.754609883378777</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>59.723328156581744</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>59.585625839143709</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>58.617002916750529</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>57.264071658810472</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>55.676311540653167</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>53.896639957984988</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>51.990082851649042</v>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>70.4731091856316</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70.5970514192686</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>70.58584182845306</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>70.5759719602495</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>70.51184704755104</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>71.10855377530721</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>71.14203826933272</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>71.03945510124709</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>70.9739407124633</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>70.84259279606606</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>70.76582444941083</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>70.84988517907877</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>70.8010545548823</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>70.61602849509131</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>70.49295396450464</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>